<commit_message>
^Update: Readme content cosmetics <chethankodenkiri>
</commit_message>
<xml_diff>
--- a/Senior Software Engineer.xlsx
+++ b/Senior Software Engineer.xlsx
@@ -43,7 +43,7 @@
     <t>Full-Stack Developer</t>
   </si>
   <si>
-    <t>https://jobs.fang.com/careerhub/explore/jobs/563156120251524</t>
+    <t>https://jobs.com/careerhub/explore/jobs/563156120251524</t>
   </si>
   <si>
     <t/>
@@ -441,7 +441,7 @@
     <col min="2" max="2" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="30.14785714285714" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="43.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="59.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">

</xml_diff>